<commit_message>
add code after recive circuit
</commit_message>
<xml_diff>
--- a/Breedlife/Tính năng phần cứng 15-10-2020.xlsx
+++ b/Breedlife/Tính năng phần cứng 15-10-2020.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ed38b5b2203511b7/Tinasoft/[BREEDLIFE] Phần mềm quản lý thiết bị/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pham Van Phuc\Desktop\breedlife\Breedlife\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="375" documentId="11_F25DC773A252ABDACC10484CA19F606E5BDE58EE" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{846F362F-671C-4D3E-8C8D-A7EFC37516C5}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-36" windowWidth="29040" windowHeight="15840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -371,7 +370,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -402,12 +401,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -465,7 +470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -521,20 +526,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -814,23 +820,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="7"/>
-    <col min="2" max="2" width="35.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="62.28515625" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="8.88671875" style="7"/>
+    <col min="2" max="2" width="35.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="39.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="62.33203125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -844,7 +850,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -856,7 +862,7 @@
       </c>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="50.4" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -868,7 +874,7 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" ht="33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -882,7 +888,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -894,7 +900,7 @@
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" ht="33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -908,7 +914,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -920,7 +926,7 @@
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -932,7 +938,7 @@
       </c>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -944,7 +950,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -956,7 +962,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -977,24 +983,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D573272-12ED-4920-9114-3C544FA0F599}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I20"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="8"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="8"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="8" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="12" max="12" width="37.140625" customWidth="1"/>
+    <col min="12" max="12" width="37.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -1014,7 +1020,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -1035,7 +1041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -1056,7 +1062,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -1077,7 +1083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -1098,7 +1104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -1119,12 +1125,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>34</v>
       </c>
@@ -1134,47 +1140,47 @@
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-    </row>
-    <row r="11" spans="1:9" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+    </row>
+    <row r="11" spans="1:9" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-    </row>
-    <row r="13" spans="1:9" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+    </row>
+    <row r="13" spans="1:9" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -1182,7 +1188,7 @@
       <c r="E14" s="9"/>
       <c r="F14" s="10"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>38</v>
       </c>
@@ -1192,67 +1198,67 @@
       <c r="E15" s="22"/>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-    </row>
-    <row r="17" spans="1:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+    </row>
+    <row r="17" spans="1:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-    </row>
-    <row r="19" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+    </row>
+    <row r="19" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="23"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A13:F13"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="A20:F20"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="A16:F16"/>
     <mergeCell ref="A17:F17"/>
     <mergeCell ref="A18:F18"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A13:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1260,26 +1266,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BF1E195-0527-45B1-8EE8-D7D8AC73FC10}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -1293,7 +1299,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="14">
         <v>1</v>
       </c>
@@ -1307,7 +1313,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="14">
         <v>2</v>
       </c>
@@ -1321,7 +1327,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="14">
         <v>3</v>
       </c>
@@ -1335,7 +1341,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="14">
         <v>4</v>
       </c>
@@ -1347,7 +1353,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="14">
         <v>5</v>
       </c>
@@ -1361,7 +1367,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="14">
         <v>6</v>
       </c>
@@ -1375,7 +1381,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="14">
         <v>7</v>
       </c>
@@ -1387,7 +1393,7 @@
       </c>
       <c r="D9" s="14"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="14">
         <v>8</v>
       </c>
@@ -1399,7 +1405,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="14">
         <v>9</v>
       </c>
@@ -1411,7 +1417,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="14">
         <v>10</v>
       </c>
@@ -1423,7 +1429,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
         <v>11</v>
       </c>
@@ -1435,7 +1441,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="14">
         <v>12</v>
       </c>
@@ -1447,7 +1453,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="14">
         <v>14</v>
       </c>
@@ -1459,7 +1465,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
         <v>15</v>
       </c>
@@ -1471,12 +1477,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
         <v>0</v>
       </c>
@@ -1490,7 +1496,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="14">
         <v>1</v>
       </c>
@@ -1502,7 +1508,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="14">
         <v>2</v>
       </c>
@@ -1516,7 +1522,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="14">
         <v>3</v>
       </c>
@@ -1530,7 +1536,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="14">
         <v>4</v>
       </c>
@@ -1549,80 +1555,80 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51771A6D-0420-4E15-96DB-967A6D4EF9D4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="41.7109375" customWidth="1"/>
-    <col min="3" max="3" width="43.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" customWidth="1"/>
+    <col min="2" max="2" width="41.6640625" customWidth="1"/>
+    <col min="3" max="3" width="43.33203125" customWidth="1"/>
+    <col min="4" max="4" width="32.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="25" t="s">
         <v>88</v>
       </c>
       <c r="C2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="25" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="25" t="s">
         <v>91</v>
       </c>
       <c r="C4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="25" t="s">
         <v>93</v>
       </c>
       <c r="C5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="25" t="s">
         <v>95</v>
       </c>
       <c r="C6" t="s">
@@ -1632,7 +1638,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1646,7 +1652,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1657,7 +1663,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1668,7 +1674,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1679,25 +1685,25 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>105</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="20" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>106</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="20" t="s">
         <v>108</v>
       </c>
     </row>

</xml_diff>